<commit_message>
folders organized; projects.json set
</commit_message>
<xml_diff>
--- a/03_design/projects.xlsx
+++ b/03_design/projects.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="-405" yWindow="30" windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Folha2" sheetId="2" r:id="rId2"/>
+    <sheet name="conversion to json" sheetId="2" r:id="rId1"/>
+    <sheet name="overall-set" sheetId="1" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$T$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'overall-set'!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="145">
   <si>
     <t>id</t>
   </si>
@@ -253,16 +253,7 @@
     <t>pInnerLink</t>
   </si>
   <si>
-    <t>Making of: https://www.youtube.com/watch?v=dCyLvDY2pSs</t>
-  </si>
-  <si>
     <t>Brief Stop-Motion Movie as a Course Final Project, about two mouses and their broken hearts made of clay.</t>
-  </si>
-  <si>
-    <t>link para ficheiro pdf</t>
-  </si>
-  <si>
-    <t>link para memoria descrititiva</t>
   </si>
   <si>
     <t>&lt;h2&gt;Introduction&lt;/h2&gt;
@@ -415,12 +406,106 @@
   <si>
     <t>project-360-tap</t>
   </si>
+  <si>
+    <t>fill-me-up</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dCyLvDY2pSs, report</t>
+  </si>
+  <si>
+    <t>projects/afghan-girl/images/1.jpg, projects/afghan-girl/images/2.jpg, projects/afghan-girl/images/3.jpg, projects/afghan-girl/images/4.jpg, projects/afghan-girl/images/1.jpg</t>
+  </si>
+  <si>
+    <t>projects/amazon-in-flames/images/1.jpg, projects/amazon-in-flames/images/2.jpg, projects/amazon-in-flames/images/3.jpg, projects/amazon-in-flames/images/4.jpg</t>
+  </si>
+  <si>
+    <t>projects/jaco-pastorius/images/1.jpg, projects/jaco-pastorius/images/2.jpg, projects/jaco-pastorius/images/3.jpg, projects/jaco-pastorius/images/4.jpg</t>
+  </si>
+  <si>
+    <t>projects/pothos/docs/brandbook-pothos.pdf</t>
+  </si>
+  <si>
+    <t>projects/pothos/images/1.jpg, projects/pothos/images/2.jpg, projects/pothos/images/3.jpg, projects/pothos/images/4.jpg, projects/pothos/images/5.jpg</t>
+  </si>
+  <si>
+    <t>projects/fill-me-up/images/1.jpg</t>
+  </si>
+  <si>
+    <t>projects/kimmidoll-haruyo/images/1.jpg, projects/kimmidoll-haruyo/images/2.jpg, projects/kimmidoll-haruyo/images/3.jpg, projects/kimmidoll-haruyo/images/4.jpg, projects/kimmidoll-haruyo/images/5.jpg</t>
+  </si>
+  <si>
+    <t>projects/musashi-tiger/images/1.jpg</t>
+  </si>
+  <si>
+    <t>projects/reativ/docs/brandbook-reativ.pdf</t>
+  </si>
+  <si>
+    <t>projects/reativ/images/1.jpg, projects/reativ/images/2.jpg, projects/reativ/images/3.jpg, projects/reativ/images/4.jpg, projects/reativ/images/5.jpg, projects/reativ/images/6.jpg, projects/reativ/images/7.jpg, projects/reativ/images/8.jpg, projects/reativ/images/9.jpg</t>
+  </si>
+  <si>
+    <t>projects/red-bull-air-race-setubal/docs/report-red-bull-air-race-setubal.pdf</t>
+  </si>
+  <si>
+    <t>projects/red-bull-air-race-setubal/images/1.jpg, projects/red-bull-air-race-setubal/images/2.jpg, projects/red-bull-air-race-setubal/images/3.jpg, projects/red-bull-air-race-setubal/images/4.jpg, projects/red-bull-air-race-setubal/images/5.jpg</t>
+  </si>
+  <si>
+    <t>projects/vinhos-e-adegas/docs/report-vinhos-setubal.pdf</t>
+  </si>
+  <si>
+    <t>projects/vinhos-e-adegas/docs/vinhos-setubal.pdf</t>
+  </si>
+  <si>
+    <t>projects/vinhos-e-adegas/images/1.jpg, projects/vinhos-e-adegas/images/2.jpg, projects/vinhos-e-adegas/images/3.jpg, projects/vinhos-e-adegas/images/4.jpg, projects/vinhos-e-adegas/images/5.jpg, projects/vinhos-e-adegas/images/6.jpg</t>
+  </si>
+  <si>
+    <t>projects/cookidoo/images/1.png</t>
+  </si>
+  <si>
+    <t>Cookidoo app improvement and Pantry Funcionality creation.</t>
+  </si>
+  <si>
+    <t>Portrait Vectorization using Adobe Flash. \n Sharbat Gula, photo by Steve McCurry.</t>
+  </si>
+  <si>
+    <t>Portrait Vectorization using Adobe Illustrator. \n Color finishing done with Adobe Photoshop. \n Jaco Pastorius, photo by Ichiro Shimizu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand Identity and Style Guide. \n Project developed for a fictional company.
+</t>
+  </si>
+  <si>
+    <t>Practical Exercise from Digital Painting Workshop. \n Part of the Graphic Design course at Flag. \n Original artwork created by instructor Ricardo Venâncio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logo Rebranding and Style Guide. \n Project developed for a real company.
+</t>
+  </si>
+  <si>
+    <t>Magazine Creation and Layout from Scratch. \n Using information and images provided on the Casa Mãe da Rota dos Vinhos website.</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Introduction&lt;/h2&gt;
+    &lt;p&gt;As part of an academic assignment to demonstrate the knowledge acquired during the Adobe InDesign layout course — provided through the FLAG training platform and taught by instructor Eduardo Antunes — students in the Graphic Design class were required to develop a project based on a magazine, following specific criteria and requirements.&lt;/p&gt;
+    &lt;p&gt;The theme of this project was left open to each student’s individual choice.&lt;/p&gt;
+    &lt;h2&gt;The Theme&lt;/h2&gt;
+    &lt;p&gt;Since I live in a rural area where vineyards are predominant — specifically in Palmela, a town well known for its wines — I chose to focus on the theme of local wines and wineries.&lt;/p&gt;
+    &lt;p&gt;After an initial research phase, I found enough information and text content to work with, particularly from the 18th Setúbal Peninsula Wine Competition:&lt;/p&gt;
+    &lt;a href="https://vinhosdapeninsuladesetubal.org\noticias/sao-56-os-melhores-vinhos-da-peninsula-de-setubal/"&gt;https://vinhosdapeninsuladesetubal.org\noticias/sao-56-os-melhores-vinhos-da-peninsula-de-setubal/&lt;/a&gt;
+    &lt;p&gt;I also drew from the Rota dos Vinhos website, a local organization based in Palmela that introduces the public — in a single space — to the products of several wineries in the Setúbal District through wine tastings and wine tourism activities:&lt;/p&gt;
+    &lt;a href="https://rotavinhospsetubal.com/adegas/"&gt;https://rotavinhospsetubal.com/adegas/&lt;/a&gt;
+    &lt;p&gt;With these resources, I was able to gather enough information about a substantial number of wineries in the region. The goal of the project was to showcase some of the wineries responsible for the award-winning wines featured in the 18th Setúbal Peninsula Wine Competition.&lt;/p&gt;
+    &lt;h2&gt;Target Audience&lt;/h2&gt;
+    &lt;p&gt;This project is aimed at a fairly specific audience, though two or three personas could be considered.&lt;/p&gt;
+    &lt;p&gt;It may be targeted at anyone who appreciates the subject — tourists or not — or at wine merchants, serving as a catalog supplement.&lt;/p&gt;
+    &lt;p&gt;The common thread is that these are adults, at least from a middle-class background, who — even though they “know what they’re looking for” — still wish to be pleasantly surprised.&lt;/p&gt;
+    &lt;p&gt;Therefore, I envisioned a visual identity for this project that is as sublime and simple as possible — striking a balance between solid graphic and design principles (albeit in a very amateur context), and a minimalist aesthetic that doesn't go overboard.&lt;/p&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,20 +514,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,12 +530,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,14 +558,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -504,9 +572,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -519,13 +584,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,9 +602,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -564,15 +626,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -865,116 +972,831 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="27" customWidth="1"/>
+    <col min="2" max="3" width="22.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="95.85546875" style="28" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="109.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="37.140625" style="39" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="65.85546875" style="39" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="23" customFormat="1">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="31" customFormat="1" ht="195">
+      <c r="A2" s="27">
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="28">
+        <v>2019</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="31" customFormat="1" ht="180">
+      <c r="A3" s="27">
+        <f>SUM(A2+1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="28">
+        <v>2020</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="31" customFormat="1" ht="180">
+      <c r="A4" s="27">
+        <f t="shared" ref="A4:A12" si="0">SUM(A3+1)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="28">
+        <v>2021</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="31" customFormat="1" ht="300">
+      <c r="A5" s="27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="28">
+        <v>2021</v>
+      </c>
+      <c r="R5" s="28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="31" customFormat="1" ht="300">
+      <c r="A6" s="27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="35">
+        <v>2021</v>
+      </c>
+      <c r="R6" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="37" customFormat="1" ht="270">
+      <c r="A7" s="27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="28">
+        <v>2022</v>
+      </c>
+      <c r="R7" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="37" customFormat="1" ht="270">
+      <c r="A8" s="27">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="28">
+        <v>2022</v>
+      </c>
+      <c r="R8" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="37" customFormat="1" ht="300">
+      <c r="A9" s="27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q9" s="28">
+        <v>2022</v>
+      </c>
+      <c r="R9" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="37" customFormat="1" ht="270">
+      <c r="A10" s="27">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O10" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="35">
+        <v>2022</v>
+      </c>
+      <c r="R10" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="37" customFormat="1" ht="405">
+      <c r="A11" s="27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O11" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="35">
+        <v>2022</v>
+      </c>
+      <c r="R11" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="37" customFormat="1" ht="165">
+      <c r="A12" s="27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="35">
+        <v>2023</v>
+      </c>
+      <c r="R12" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="28"/>
+      <c r="D13" s="39"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="28"/>
+      <c r="P13" s="39"/>
+      <c r="R13" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="17" customWidth="1"/>
     <col min="4" max="5" width="22.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="109.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="37.140625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="109.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="37.140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="65.85546875" style="6" customWidth="1"/>
     <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="21" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:20" s="19" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="195">
+      <c r="A2" s="7">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" s="23" t="s">
+      <c r="D2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="T1" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="195">
-      <c r="A2" s="8">
-        <v>0</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>110</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>50</v>
@@ -1000,10 +1822,10 @@
       <c r="N2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>67</v>
       </c>
       <c r="Q2" s="3" t="s">
@@ -1015,23 +1837,25 @@
       <c r="S2" s="3">
         <v>2019</v>
       </c>
-      <c r="T2" s="3"/>
+      <c r="T2" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="180">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>105</v>
+      <c r="B3" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>111</v>
+        <v>82</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>72</v>
@@ -1060,10 +1884,10 @@
       <c r="N3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="8" t="s">
         <v>66</v>
       </c>
       <c r="Q3" s="3" t="s">
@@ -1072,28 +1896,28 @@
       <c r="R3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="5">
         <v>2019</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="18" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" ht="180">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>105</v>
+      <c r="B4" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>112</v>
+        <v>89</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>21</v>
@@ -1122,10 +1946,10 @@
       <c r="N4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="8" t="s">
         <v>66</v>
       </c>
       <c r="Q4" s="3" t="s">
@@ -1137,26 +1961,28 @@
       <c r="S4" s="3">
         <v>2020</v>
       </c>
-      <c r="T4" s="3"/>
+      <c r="T4" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="5" spans="1:20" s="1" customFormat="1" ht="180">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>105</v>
+      <c r="B5" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>113</v>
+        <v>90</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>47</v>
@@ -1176,14 +2002,14 @@
       <c r="N5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="8" t="s">
         <v>66</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>24</v>
@@ -1191,22 +2017,24 @@
       <c r="S5" s="3">
         <v>2021</v>
       </c>
-      <c r="T5" s="3"/>
+      <c r="T5" s="3" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="6" spans="1:20" s="1" customFormat="1" ht="300">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>105</v>
+      <c r="B6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1227,20 +2055,20 @@
       <c r="K6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M6" s="3" t="s">
+      <c r="L6" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>72</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="9" t="s">
-        <v>84</v>
+      <c r="P6" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>12</v>
@@ -1251,28 +2079,30 @@
       <c r="S6" s="3">
         <v>2021</v>
       </c>
-      <c r="T6" s="3"/>
+      <c r="T6" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:20" s="1" customFormat="1" ht="300">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="E7" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -1282,51 +2112,55 @@
         <v>72</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>74</v>
+        <v>86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" t="s">
         <v>29</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="8" t="s">
         <v>66</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="S7" s="6">
+        <v>77</v>
+      </c>
+      <c r="S7" s="5">
         <v>2021</v>
       </c>
-      <c r="T7" s="4"/>
+      <c r="T7" s="18" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="8" spans="1:20" s="1" customFormat="1" ht="195">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>105</v>
+      <c r="B8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="F8" s="3" t="s">
         <v>72</v>
       </c>
@@ -1354,19 +2188,19 @@
       <c r="N8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="8" t="s">
         <v>67</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="5">
         <v>2021</v>
       </c>
       <c r="T8" s="3" t="s">
@@ -1374,20 +2208,20 @@
       </c>
     </row>
     <row r="9" spans="1:20" s="2" customFormat="1" ht="195">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>105</v>
+      <c r="B9" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>72</v>
@@ -1416,19 +2250,19 @@
       <c r="N9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="8" t="s">
         <v>67</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="5">
         <v>2021</v>
       </c>
       <c r="T9" s="3" t="s">
@@ -1436,20 +2270,20 @@
       </c>
     </row>
     <row r="10" spans="1:20" s="2" customFormat="1" ht="270">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>105</v>
+      <c r="B10" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>117</v>
+        <v>83</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>35</v>
@@ -1478,10 +2312,10 @@
       <c r="N10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" t="s">
         <v>43</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="9" t="s">
         <v>64</v>
       </c>
       <c r="Q10" s="3" t="s">
@@ -1493,23 +2327,25 @@
       <c r="S10" s="3">
         <v>2022</v>
       </c>
-      <c r="T10" s="3"/>
+      <c r="T10" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="11" spans="1:20" s="2" customFormat="1" ht="270">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>105</v>
+      <c r="B11" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>118</v>
+        <v>92</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>30</v>
@@ -1538,10 +2374,10 @@
       <c r="N11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" t="s">
         <v>27</v>
       </c>
-      <c r="P11" s="11" t="s">
+      <c r="P11" s="10" t="s">
         <v>64</v>
       </c>
       <c r="Q11" s="3" t="s">
@@ -1553,28 +2389,30 @@
       <c r="S11" s="3">
         <v>2022</v>
       </c>
-      <c r="T11" s="3"/>
+      <c r="T11" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="12" spans="1:20" s="2" customFormat="1" ht="300">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>105</v>
+      <c r="B12" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>57</v>
       </c>
       <c r="H12" s="3" t="s">
@@ -1589,8 +2427,8 @@
       <c r="K12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>72</v>
+      <c r="L12" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>72</v>
@@ -1598,10 +2436,10 @@
       <c r="N12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" t="s">
         <v>28</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="P12" s="8" t="s">
         <v>65</v>
       </c>
       <c r="Q12" s="3" t="s">
@@ -1613,23 +2451,25 @@
       <c r="S12" s="3">
         <v>2022</v>
       </c>
-      <c r="T12" s="3"/>
+      <c r="T12" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="13" spans="1:20" s="2" customFormat="1" ht="270">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>105</v>
+      <c r="B13" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>69</v>
@@ -1646,8 +2486,8 @@
       <c r="J13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>72</v>
+      <c r="K13" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>72</v>
@@ -1658,10 +2498,10 @@
       <c r="N13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" t="s">
         <v>43</v>
       </c>
-      <c r="P13" s="11" t="s">
+      <c r="P13" s="10" t="s">
         <v>64</v>
       </c>
       <c r="Q13" s="3" t="s">
@@ -1670,26 +2510,28 @@
       <c r="R13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="5">
         <v>2022</v>
       </c>
-      <c r="T13" s="6"/>
+      <c r="T13" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="14" spans="1:20" s="2" customFormat="1" ht="405">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>12</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>106</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>120</v>
+        <v>95</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>19</v>
@@ -1704,49 +2546,53 @@
         <v>72</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" t="s">
         <v>43</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="P14" s="10" t="s">
         <v>64</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S14" s="6">
+      <c r="S14" s="5">
         <v>2022</v>
       </c>
-      <c r="T14" s="6"/>
+      <c r="T14" s="3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="15" spans="1:20" s="2" customFormat="1" ht="165">
-      <c r="A15" s="12">
+      <c r="A15" s="11">
         <v>13</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>105</v>
+      <c r="B15" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -1756,7 +2602,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>62</v>
@@ -1764,18 +2610,18 @@
       <c r="J15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="4" t="s">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" t="s">
         <v>37</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" t="s">
         <v>42</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="P15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="Q15" s="3" t="s">
@@ -1784,26 +2630,28 @@
       <c r="R15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="5">
         <v>2023</v>
       </c>
-      <c r="T15" s="6"/>
+      <c r="T15" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="16" spans="1:20" s="2" customFormat="1" ht="120">
-      <c r="A16" s="13">
+      <c r="A16" s="12">
         <v>14</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>105</v>
+      <c r="B16" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>121</v>
+        <v>97</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>72</v>
@@ -1832,10 +2680,10 @@
       <c r="N16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O16" s="4" t="s">
+      <c r="O16" t="s">
         <v>42</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="8" t="s">
         <v>68</v>
       </c>
       <c r="Q16" s="3" t="s">
@@ -1844,19 +2692,21 @@
       <c r="R16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S16" s="6">
+      <c r="S16" s="5">
         <v>2023</v>
       </c>
-      <c r="T16" s="6"/>
+      <c r="T16" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="3"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="F17" s="7"/>
-      <c r="O17" s="10"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="F17" s="6"/>
+      <c r="O17" s="9"/>
       <c r="P17" s="3"/>
-      <c r="R17" s="7"/>
+      <c r="R17" s="6"/>
       <c r="T17"/>
     </row>
   </sheetData>
@@ -1868,39 +2718,8 @@
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
-  <hyperlinks>
-    <hyperlink ref="O11" r:id="rId1"/>
-    <hyperlink ref="O12" r:id="rId2"/>
-    <hyperlink ref="M7" r:id="rId3"/>
-    <hyperlink ref="M15" r:id="rId4"/>
-    <hyperlink ref="O15" r:id="rId5"/>
-    <hyperlink ref="O16" r:id="rId6"/>
-    <hyperlink ref="O14" r:id="rId7"/>
-    <hyperlink ref="O10" r:id="rId8"/>
-    <hyperlink ref="O13" r:id="rId9"/>
-    <hyperlink ref="O4" r:id="rId10"/>
-    <hyperlink ref="O5" r:id="rId11"/>
-    <hyperlink ref="O2" r:id="rId12"/>
-    <hyperlink ref="O6" r:id="rId13"/>
-    <hyperlink ref="O7" r:id="rId14"/>
-    <hyperlink ref="O8" r:id="rId15"/>
-    <hyperlink ref="O9" r:id="rId16"/>
-    <hyperlink ref="O3" r:id="rId17"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
filtros actualizados; .json actualizados
</commit_message>
<xml_diff>
--- a/03_design/projects.xlsx
+++ b/03_design/projects.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="155">
   <si>
     <t>id</t>
   </si>
@@ -499,6 +499,36 @@
     &lt;p&gt;It may be targeted at anyone who appreciates the subject — tourists or not — or at wine merchants, serving as a catalog supplement.&lt;/p&gt;
     &lt;p&gt;The common thread is that these are adults, at least from a middle-class background, who — even though they “know what they’re looking for” — still wish to be pleasantly surprised.&lt;/p&gt;
     &lt;p&gt;Therefore, I envisioned a visual identity for this project that is as sublime and simple as possible — striking a balance between solid graphic and design principles (albeit in a very amateur context), and a minimalist aesthetic that doesn't go overboard.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>illustration,  Flag, academic</t>
+  </si>
+  <si>
+    <t>branding, , IEFP Setubal, academic</t>
+  </si>
+  <si>
+    <t>illustration,  IEFP Setubal, academic</t>
+  </si>
+  <si>
+    <t>illustration, IEFP Setubal, academic</t>
+  </si>
+  <si>
+    <t>Video, IEFP Setubal, academic, internship</t>
+  </si>
+  <si>
+    <t>packaging, Flag, academic</t>
+  </si>
+  <si>
+    <t>branding, Flag, academic</t>
+  </si>
+  <si>
+    <t>communication design, Flag, academic</t>
+  </si>
+  <si>
+    <t>editorial design, Flag, academic</t>
+  </si>
+  <si>
+    <t>ux/ui desgin, edit, academic</t>
   </si>
 </sst>
 </file>
@@ -520,7 +550,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +560,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -677,6 +713,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="J12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1103,7 +1142,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="28" t="s">
-        <v>24</v>
+        <v>148</v>
       </c>
       <c r="Q2" s="28">
         <v>2019</v>
@@ -1160,7 +1199,7 @@
         <v>13</v>
       </c>
       <c r="P3" s="28" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="Q3" s="28">
         <v>2020</v>
@@ -1211,7 +1250,7 @@
         <v>80</v>
       </c>
       <c r="P4" s="28" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="Q4" s="28">
         <v>2021</v>
@@ -1268,7 +1307,7 @@
         <v>12</v>
       </c>
       <c r="P5" s="28" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="Q5" s="28">
         <v>2021</v>
@@ -1324,8 +1363,8 @@
       <c r="O6" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="28" t="s">
-        <v>77</v>
+      <c r="P6" s="40" t="s">
+        <v>149</v>
       </c>
       <c r="Q6" s="35">
         <v>2021</v>
@@ -1382,7 +1421,7 @@
         <v>12</v>
       </c>
       <c r="P7" s="28" t="s">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="Q7" s="28">
         <v>2022</v>
@@ -1439,7 +1478,7 @@
         <v>13</v>
       </c>
       <c r="P8" s="28" t="s">
-        <v>24</v>
+        <v>145</v>
       </c>
       <c r="Q8" s="28">
         <v>2022</v>
@@ -1496,7 +1535,7 @@
         <v>12</v>
       </c>
       <c r="P9" s="28" t="s">
-        <v>24</v>
+        <v>151</v>
       </c>
       <c r="Q9" s="28">
         <v>2022</v>
@@ -1553,7 +1592,7 @@
         <v>13</v>
       </c>
       <c r="P10" s="28" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="Q10" s="35">
         <v>2022</v>
@@ -1610,7 +1649,7 @@
         <v>78</v>
       </c>
       <c r="P11" s="28" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
       <c r="Q11" s="35">
         <v>2022</v>
@@ -1663,7 +1702,7 @@
         <v>25</v>
       </c>
       <c r="P12" s="28" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="Q12" s="35">
         <v>2023</v>
@@ -1682,6 +1721,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>